<commit_message>
added HUQ051 to questionnaire
</commit_message>
<xml_diff>
--- a/Data/Cancer Crosswalk.xlsx
+++ b/Data/Cancer Crosswalk.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://huroncg-my.sharepoint.com/personal/khirst_huronconsultinggroup_com/Documents/Desktop/RPA/VA Project/ML_RPA_Use_Cases/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="145" documentId="8_{94D74047-659A-44CD-9B26-E5C8751BFCAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC4964E9-CBCA-401C-BEA2-AB9F46C61D24}"/>
+  <xr:revisionPtr revIDLastSave="186" documentId="8_{94D74047-659A-44CD-9B26-E5C8751BFCAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94426101-4908-436E-B8A5-139A5DB7E524}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="7710" windowWidth="29040" windowHeight="17640" activeTab="6" xr2:uid="{D1BD660C-3ABA-47D9-B6C9-7B11077B7DA9}"/>
   </bookViews>
@@ -19,11 +19,12 @@
     <sheet name="MCQ560" sheetId="4" r:id="rId4"/>
     <sheet name="MCQ371D" sheetId="5" r:id="rId5"/>
     <sheet name="HUQ071" sheetId="6" r:id="rId6"/>
-    <sheet name="OHQ033" sheetId="7" r:id="rId7"/>
-    <sheet name="MCQ092" sheetId="8" r:id="rId8"/>
-    <sheet name="SMQ020" sheetId="9" r:id="rId9"/>
-    <sheet name="DPQ040" sheetId="10" r:id="rId10"/>
-    <sheet name="PUQ110" sheetId="11" r:id="rId11"/>
+    <sheet name="HUQ051" sheetId="12" r:id="rId7"/>
+    <sheet name="OHQ033" sheetId="7" r:id="rId8"/>
+    <sheet name="MCQ092" sheetId="8" r:id="rId9"/>
+    <sheet name="SMQ020" sheetId="9" r:id="rId10"/>
+    <sheet name="DPQ040" sheetId="10" r:id="rId11"/>
+    <sheet name="PUQ110" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="37">
   <si>
     <t>Yes</t>
   </si>
@@ -127,6 +128,36 @@
   </si>
   <si>
     <t>Nearly every day</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>2 to 3</t>
+  </si>
+  <si>
+    <t>4 to 5</t>
+  </si>
+  <si>
+    <t>6 to 7</t>
+  </si>
+  <si>
+    <t>8 to 9</t>
+  </si>
+  <si>
+    <t>10 to 12</t>
+  </si>
+  <si>
+    <t>13 to 15</t>
+  </si>
+  <si>
+    <t>16 or more</t>
+  </si>
+  <si>
+    <t>Don’t Know</t>
   </si>
 </sst>
 </file>
@@ -191,6 +222,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -482,7 +517,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -556,6 +591,69 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{805B6E7C-AFB8-4CFD-8237-93E1AF6AAF97}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E823BED7-41F2-4E4E-9EE3-1F2D2EF885DB}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -637,7 +735,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51B0C6DD-7C50-4C21-8D43-16D18EF3747E}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -705,7 +803,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1078,10 +1176,132 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A2CADE-25FD-4953-9151-4F2538EB0849}">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <cols>
+    <col min="2" max="2" width="10.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6496823C-C4A7-447B-ADFA-5FBA45C92B1F}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1167,7 +1387,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA57E32-BA7B-4DB1-B818-AA9F27B1C077}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1228,67 +1448,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{805B6E7C-AFB8-4CFD-8237-93E1AF6AAF97}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>